<commit_message>
Ny test optimal OOS
</commit_message>
<xml_diff>
--- a/Input_data_With_dummyGrid_and_RT.xlsx
+++ b/Input_data_With_dummyGrid_and_RT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Simple_extended\Out_of_sample_alu\Max_case_alu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFB02F0-5B37-4AA2-970F-45DE60B0CB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C638CBEC-E541-431E-B90E-B5E658926DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="16" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="14" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_AvailableExcessHeat" sheetId="8" r:id="rId1"/>
@@ -3041,8 +3041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3083,7 +3083,7 @@
         <v>60</v>
       </c>
       <c r="B5">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3091,7 +3091,7 @@
         <v>72</v>
       </c>
       <c r="B6">
-        <v>1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3235,8 +3235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3952,7 +3952,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4010,7 +4010,7 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4047,7 +4047,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4105,7 +4105,7 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -6692,26 +6692,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEBC57C6511F094FB1659D4FD897CA2A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e300c8dce90f4bd359ffe07958d068a6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5caa653f-10d0-46a2-81cc-01cb3798075e" xmlns:ns3="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="947f29ac9f688054ae1e7aaca14544db" ns2:_="" ns3:_="">
     <xsd:import namespace="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
@@ -6912,10 +6892,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07060BB5-5F94-4742-B93F-B4D1C211ED2E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
+    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6938,20 +6949,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07060BB5-5F94-4742-B93F-B4D1C211ED2E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
-    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>